<commit_message>
Matrices de migración reciente 2015 e indicadores
</commit_message>
<xml_diff>
--- a/Resumen/2020/Entidad/01 Migración reciente 2015 - 2020/Matriz de migracion reciente a nivel estatal 2015-2020.xlsx
+++ b/Resumen/2020/Entidad/01 Migración reciente 2015 - 2020/Matriz de migracion reciente a nivel estatal 2015-2020.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prontuario_migracion_interna\Resumen\2020\Entidad\01 Migración reciente 2005 - 2010\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prontuario_migracion_interna\Resumen\2020\Entidad\01 Migración reciente 2015 - 2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3475A6B2-9589-4931-8F7C-DABAF981CE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DE1E3B-C564-4624-88DC-4B3BAEBB500D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34452" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MREst. 2015-2020" sheetId="1" r:id="rId1"/>
     <sheet name="Indicadores" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="81">
   <si>
     <t>Aguascalientes</t>
   </si>
@@ -328,15 +341,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -430,6 +434,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -452,6 +465,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -473,18 +489,8 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -493,7 +499,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -511,13 +517,20 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -818,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B37"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.45"/>
@@ -836,20 +849,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>68</v>
       </c>
     </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="4" spans="1:34" ht="12.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:34" s="6" customFormat="1" ht="36.4" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
@@ -4291,10 +4309,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FDB9E2-05DF-45E7-8E0E-ACC38131F440}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4307,1212 +4325,1223 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A2" s="21"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="1:11" ht="42" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="22" t="s">
+      <c r="A2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:11" ht="14.65" x14ac:dyDescent="0.5">
+      <c r="A3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:11" ht="42" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D4" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E4" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F4" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G4" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H4" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I4" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J4" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K4" s="19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="23" t="s">
+    <row r="5" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B5" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C5" s="5">
         <v>125515554</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D5" s="5">
         <v>115392501</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E5" s="5">
         <v>110724958</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F5" s="5">
         <v>3936679</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G5" s="5">
         <v>3936679</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H5" s="5">
         <v>565844</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I5" s="5">
         <v>32564</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J5" s="5">
         <v>1461</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K5" s="5">
         <v>130995</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" s="25" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B6" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C6" s="24">
         <v>1421198</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D6" s="24">
         <v>1296230</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E6" s="24">
         <v>1226454</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F6" s="24">
         <v>60587</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G6" s="24">
         <v>24773</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H6" s="24">
         <v>8931</v>
       </c>
-      <c r="I5" s="27">
+      <c r="I6" s="24">
         <v>48</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J6" s="24">
         <v>0</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K6" s="24">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" s="25" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C7" s="24">
         <v>3739797</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D7" s="24">
         <v>3464891</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E7" s="24">
         <v>3155213</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F7" s="24">
         <v>249358</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G7" s="24">
         <v>91483</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H7" s="24">
         <v>53942</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I7" s="24">
         <v>1097</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J7" s="24">
         <v>90</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K7" s="24">
         <v>5191</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" s="25" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C8" s="24">
         <v>793424</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D8" s="24">
         <v>729216</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E8" s="24">
         <v>655361</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F8" s="24">
         <v>68474</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G8" s="24">
         <v>32497</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H8" s="24">
         <v>4064</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I8" s="24">
         <v>365</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J8" s="24">
         <v>0</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K8" s="24">
         <v>952</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" s="25" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C9" s="24">
         <v>926858</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D9" s="24">
         <v>848445</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E9" s="24">
         <v>795746</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F9" s="24">
         <v>35515</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G9" s="24">
         <v>51028</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H9" s="24">
         <v>2683</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I9" s="24">
         <v>142</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J9" s="24">
         <v>0</v>
       </c>
-      <c r="K8" s="27">
+      <c r="K9" s="24">
         <v>14359</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" s="25" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C10" s="24">
         <v>3137032</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D10" s="24">
         <v>2855617</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E10" s="24">
         <v>2761903</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F10" s="24">
         <v>77049</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G10" s="24">
         <v>63950</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H10" s="24">
         <v>13116</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I10" s="24">
         <v>641</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J10" s="24">
         <v>116</v>
       </c>
-      <c r="K9" s="27">
+      <c r="K10" s="24">
         <v>2792</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" s="25" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C11" s="24">
         <v>728300</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D11" s="24">
         <v>674851</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E11" s="24">
         <v>633038</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F11" s="24">
         <v>37334</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G11" s="24">
         <v>29755</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H11" s="24">
         <v>4331</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I11" s="24">
         <v>31</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J11" s="24">
         <v>0</v>
       </c>
-      <c r="K10" s="27">
+      <c r="K11" s="24">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" s="25" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B12" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C12" s="24">
         <v>5524506</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D12" s="24">
         <v>4938226</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E12" s="24">
         <v>4849943</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F12" s="24">
         <v>55455</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G12" s="24">
         <v>167279</v>
       </c>
-      <c r="H11" s="27">
+      <c r="H12" s="24">
         <v>21811</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I12" s="24">
         <v>402</v>
       </c>
-      <c r="J11" s="27">
+      <c r="J12" s="24">
         <v>123</v>
       </c>
-      <c r="K11" s="27">
+      <c r="K12" s="24">
         <v>10492</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12" s="25" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B13" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C13" s="24">
         <v>3725058</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D13" s="24">
         <v>3427399</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E13" s="24">
         <v>3287846</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F13" s="24">
         <v>108985</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G13" s="24">
         <v>65187</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H13" s="24">
         <v>27344</v>
       </c>
-      <c r="I12" s="27">
+      <c r="I13" s="24">
         <v>739</v>
       </c>
-      <c r="J12" s="27">
+      <c r="J13" s="24">
         <v>139</v>
       </c>
-      <c r="K12" s="27">
+      <c r="K13" s="24">
         <v>2346</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13" s="25" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B14" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C14" s="24">
         <v>9159393</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D14" s="24">
         <v>8675781</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E14" s="24">
         <v>8274545</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F14" s="24">
         <v>338196</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G14" s="24">
         <v>566115</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H14" s="24">
         <v>50006</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I14" s="24">
         <v>4134</v>
       </c>
-      <c r="J13" s="27">
+      <c r="J14" s="24">
         <v>415</v>
       </c>
-      <c r="K13" s="27">
+      <c r="K14" s="24">
         <v>8485</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A14" s="25" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B15" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C15" s="24">
         <v>1821279</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D15" s="24">
         <v>1652979</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E15" s="24">
         <v>1598892</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F15" s="24">
         <v>43652</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G15" s="24">
         <v>56889</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H15" s="24">
         <v>9826</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I15" s="24">
         <v>99</v>
       </c>
-      <c r="J14" s="27">
+      <c r="J15" s="24">
         <v>2</v>
       </c>
-      <c r="K14" s="27">
+      <c r="K15" s="24">
         <v>508</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A15" s="25" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B16" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C16" s="24">
         <v>6144449</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D16" s="24">
         <v>5598366</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E16" s="24">
         <v>5459604</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F16" s="24">
         <v>104757</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G16" s="24">
         <v>93369</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H16" s="24">
         <v>27045</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I16" s="24">
         <v>1475</v>
       </c>
-      <c r="J15" s="27">
+      <c r="J16" s="24">
         <v>33</v>
       </c>
-      <c r="K15" s="27">
+      <c r="K16" s="24">
         <v>5452</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16" s="25" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A17" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B17" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C17" s="24">
         <v>3525695</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D17" s="24">
         <v>3187065</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E17" s="24">
         <v>3111059</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F17" s="24">
         <v>61652</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G17" s="24">
         <v>187853</v>
       </c>
-      <c r="H16" s="27">
+      <c r="H17" s="24">
         <v>12733</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I17" s="24">
         <v>301</v>
       </c>
-      <c r="J16" s="27">
+      <c r="J17" s="24">
         <v>3</v>
       </c>
-      <c r="K16" s="27">
+      <c r="K17" s="24">
         <v>1317</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A17" s="25" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A18" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B18" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C18" s="24">
         <v>3075237</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D18" s="24">
         <v>2836379</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E18" s="24">
         <v>2665783</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F18" s="24">
         <v>156179</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G18" s="24">
         <v>87173</v>
       </c>
-      <c r="H17" s="27">
+      <c r="H18" s="24">
         <v>12914</v>
       </c>
-      <c r="I17" s="27">
+      <c r="I18" s="24">
         <v>299</v>
       </c>
-      <c r="J17" s="27">
+      <c r="J18" s="24">
         <v>0</v>
       </c>
-      <c r="K17" s="27">
+      <c r="K18" s="24">
         <v>1204</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A18" s="25" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A19" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C19" s="24">
         <v>8303835</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D19" s="24">
         <v>7626435</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E19" s="24">
         <v>7375857</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F19" s="24">
         <v>198977</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G19" s="24">
         <v>162934</v>
       </c>
-      <c r="H18" s="27">
+      <c r="H19" s="24">
         <v>44354</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I19" s="24">
         <v>1308</v>
       </c>
-      <c r="J18" s="27">
+      <c r="J19" s="24">
         <v>116</v>
       </c>
-      <c r="K18" s="27">
+      <c r="K19" s="24">
         <v>5823</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A19" s="25" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C20" s="24">
         <v>16943627</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D20" s="24">
         <v>15661775</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E20" s="24">
         <v>15154946</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F20" s="24">
         <v>450751</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G20" s="24">
         <v>520719</v>
       </c>
-      <c r="H19" s="27">
+      <c r="H20" s="24">
         <v>30836</v>
       </c>
-      <c r="I19" s="27">
+      <c r="I20" s="24">
         <v>10067</v>
       </c>
-      <c r="J19" s="27">
+      <c r="J20" s="24">
         <v>231</v>
       </c>
-      <c r="K19" s="27">
+      <c r="K20" s="24">
         <v>14944</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A20" s="25" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B21" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C21" s="24">
         <v>4728162</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D21" s="24">
         <v>4298137</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E21" s="24">
         <v>4170781</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F21" s="24">
         <v>94667</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G21" s="24">
         <v>116732</v>
       </c>
-      <c r="H20" s="27">
+      <c r="H21" s="24">
         <v>29259</v>
       </c>
-      <c r="I20" s="27">
+      <c r="I21" s="24">
         <v>677</v>
       </c>
-      <c r="J20" s="27">
+      <c r="J21" s="24">
         <v>0</v>
       </c>
-      <c r="K20" s="27">
+      <c r="K21" s="24">
         <v>2753</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A21" s="25" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B22" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C22" s="24">
         <v>1961694</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D22" s="24">
         <v>1816739</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E22" s="24">
         <v>1714221</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F22" s="24">
         <v>90214</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G22" s="24">
         <v>66942</v>
       </c>
-      <c r="H21" s="27">
+      <c r="H22" s="24">
         <v>9866</v>
       </c>
-      <c r="I21" s="27">
+      <c r="I22" s="24">
         <v>135</v>
       </c>
-      <c r="J21" s="27">
+      <c r="J22" s="24">
         <v>24</v>
       </c>
-      <c r="K21" s="27">
+      <c r="K22" s="24">
         <v>2279</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A22" s="25" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B23" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C23" s="24">
         <v>1226179</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D23" s="24">
         <v>1123645</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E23" s="24">
         <v>1069488</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F23" s="24">
         <v>46167</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G23" s="24">
         <v>41791</v>
       </c>
-      <c r="H22" s="27">
+      <c r="H23" s="24">
         <v>7375</v>
       </c>
-      <c r="I22" s="27">
+      <c r="I23" s="24">
         <v>179</v>
       </c>
-      <c r="J22" s="27">
+      <c r="J23" s="24">
         <v>4</v>
       </c>
-      <c r="K22" s="27">
+      <c r="K23" s="24">
         <v>432</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A23" s="25" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A24" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B24" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C24" s="24">
         <v>5768781</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D24" s="24">
         <v>5314945</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E24" s="24">
         <v>5004402</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F24" s="24">
         <v>270744</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G24" s="24">
         <v>93008</v>
       </c>
-      <c r="H23" s="27">
+      <c r="H24" s="24">
         <v>24771</v>
       </c>
-      <c r="I23" s="27">
+      <c r="I24" s="24">
         <v>2762</v>
       </c>
-      <c r="J23" s="27">
+      <c r="J24" s="24">
         <v>104</v>
       </c>
-      <c r="K23" s="27">
+      <c r="K24" s="24">
         <v>12162</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A24" s="25" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A25" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B25" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="27">
+      <c r="C25" s="24">
         <v>4113433</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D25" s="24">
         <v>3751736</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E25" s="24">
         <v>3635167</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F25" s="24">
         <v>95409</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G25" s="24">
         <v>136116</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H25" s="24">
         <v>19238</v>
       </c>
-      <c r="I24" s="27">
+      <c r="I25" s="24">
         <v>678</v>
       </c>
-      <c r="J24" s="27">
+      <c r="J25" s="24">
         <v>13</v>
       </c>
-      <c r="K24" s="27">
+      <c r="K25" s="24">
         <v>1231</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A25" s="25" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A26" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B26" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="27">
+      <c r="C26" s="24">
         <v>6567595</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D26" s="24">
         <v>5980199</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E26" s="24">
         <v>5778654</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F26" s="24">
         <v>176573</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G26" s="24">
         <v>161667</v>
       </c>
-      <c r="H25" s="27">
+      <c r="H26" s="24">
         <v>21283</v>
       </c>
-      <c r="I25" s="27">
+      <c r="I26" s="24">
         <v>1106</v>
       </c>
-      <c r="J25" s="27">
+      <c r="J26" s="24">
         <v>2</v>
       </c>
-      <c r="K25" s="27">
+      <c r="K26" s="24">
         <v>2581</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A26" s="25" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A27" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B27" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="27">
+      <c r="C27" s="24">
         <v>2362209</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D27" s="24">
         <v>2176868</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E27" s="24">
         <v>1969009</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F27" s="24">
         <v>192057</v>
       </c>
-      <c r="G26" s="27">
+      <c r="G27" s="24">
         <v>61615</v>
       </c>
-      <c r="H26" s="27">
+      <c r="H27" s="24">
         <v>13680</v>
       </c>
-      <c r="I26" s="27">
+      <c r="I27" s="24">
         <v>850</v>
       </c>
-      <c r="J26" s="27">
+      <c r="J27" s="24">
         <v>0</v>
       </c>
-      <c r="K26" s="27">
+      <c r="K27" s="24">
         <v>1272</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A27" s="25" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A28" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B28" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C28" s="24">
         <v>1852929</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D28" s="24">
         <v>1702045</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E28" s="24">
         <v>1491918</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F28" s="24">
         <v>191167</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G28" s="24">
         <v>82718</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H28" s="24">
         <v>15398</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I28" s="24">
         <v>612</v>
       </c>
-      <c r="J27" s="27">
+      <c r="J28" s="24">
         <v>0</v>
       </c>
-      <c r="K27" s="27">
+      <c r="K28" s="24">
         <v>2950</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A28" s="25" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B29" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="27">
+      <c r="C29" s="24">
         <v>2815438</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D29" s="24">
         <v>2585174</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E29" s="24">
         <v>2506515</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F29" s="24">
         <v>60020</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G29" s="24">
         <v>68051</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H29" s="24">
         <v>14998</v>
       </c>
-      <c r="I28" s="27">
+      <c r="I29" s="24">
         <v>1583</v>
       </c>
-      <c r="J28" s="27">
+      <c r="J29" s="24">
         <v>26</v>
       </c>
-      <c r="K28" s="27">
+      <c r="K29" s="24">
         <v>2032</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A29" s="25" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B30" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="27">
+      <c r="C30" s="24">
         <v>2986880</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D30" s="24">
         <v>2751749</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E30" s="24">
         <v>2657941</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F30" s="24">
         <v>84168</v>
       </c>
-      <c r="G29" s="27">
+      <c r="G30" s="24">
         <v>108843</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H30" s="24">
         <v>8227</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I30" s="24">
         <v>346</v>
       </c>
-      <c r="J29" s="27">
+      <c r="J30" s="24">
         <v>0</v>
       </c>
-      <c r="K29" s="27">
+      <c r="K30" s="24">
         <v>1067</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A30" s="25" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A31" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B31" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="27">
+      <c r="C31" s="24">
         <v>2924652</v>
       </c>
-      <c r="D30" s="27">
+      <c r="D31" s="24">
         <v>2703869</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E31" s="24">
         <v>2620188</v>
       </c>
-      <c r="F30" s="27">
+      <c r="F31" s="24">
         <v>66694</v>
       </c>
-      <c r="G30" s="27">
+      <c r="G31" s="24">
         <v>65096</v>
       </c>
-      <c r="H30" s="27">
+      <c r="H31" s="24">
         <v>14061</v>
       </c>
-      <c r="I30" s="27">
+      <c r="I31" s="24">
         <v>519</v>
       </c>
-      <c r="J30" s="27">
+      <c r="J31" s="24">
         <v>19</v>
       </c>
-      <c r="K30" s="27">
+      <c r="K31" s="24">
         <v>2388</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A31" s="25" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A32" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B32" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="27">
+      <c r="C32" s="24">
         <v>2397125</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D32" s="24">
         <v>2188340</v>
       </c>
-      <c r="E31" s="27">
+      <c r="E32" s="24">
         <v>2136340</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F32" s="24">
         <v>47562</v>
       </c>
-      <c r="G31" s="27">
+      <c r="G32" s="24">
         <v>120484</v>
       </c>
-      <c r="H31" s="27">
+      <c r="H32" s="24">
         <v>4008</v>
       </c>
-      <c r="I31" s="27">
+      <c r="I32" s="24">
         <v>140</v>
       </c>
-      <c r="J31" s="27">
+      <c r="J32" s="24">
         <v>0</v>
       </c>
-      <c r="K31" s="27">
+      <c r="K32" s="24">
         <v>290</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A32" s="25" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A33" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B33" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="27">
+      <c r="C33" s="24">
         <v>3518497</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D33" s="24">
         <v>3244697</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E33" s="24">
         <v>3116244</v>
       </c>
-      <c r="F32" s="27">
+      <c r="F33" s="24">
         <v>108145</v>
       </c>
-      <c r="G32" s="27">
+      <c r="G33" s="24">
         <v>109605</v>
       </c>
-      <c r="H32" s="27">
+      <c r="H33" s="24">
         <v>17963</v>
       </c>
-      <c r="I32" s="27">
+      <c r="I33" s="24">
         <v>629</v>
       </c>
-      <c r="J32" s="27">
+      <c r="J33" s="24">
         <v>0</v>
       </c>
-      <c r="K32" s="27">
+      <c r="K33" s="24">
         <v>1716</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A33" s="25" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A34" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B34" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="27">
+      <c r="C34" s="24">
         <v>1340912</v>
       </c>
-      <c r="D33" s="27">
+      <c r="D34" s="24">
         <v>1228497</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E34" s="24">
         <v>1163828</v>
       </c>
-      <c r="F33" s="27">
+      <c r="F34" s="24">
         <v>43476</v>
       </c>
-      <c r="G33" s="27">
+      <c r="G34" s="24">
         <v>29192</v>
       </c>
-      <c r="H33" s="27">
+      <c r="H34" s="24">
         <v>3304</v>
       </c>
-      <c r="I33" s="27">
+      <c r="I34" s="24">
         <v>84</v>
       </c>
-      <c r="J33" s="27">
+      <c r="J34" s="24">
         <v>0</v>
       </c>
-      <c r="K33" s="27">
+      <c r="K34" s="24">
         <v>17805</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A34" s="25" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A35" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B35" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="27">
+      <c r="C35" s="24">
         <v>8046861</v>
       </c>
-      <c r="D34" s="27">
+      <c r="D35" s="24">
         <v>7444681</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E35" s="24">
         <v>7253629</v>
       </c>
-      <c r="F34" s="27">
+      <c r="F35" s="24">
         <v>169749</v>
       </c>
-      <c r="G34" s="27">
+      <c r="G35" s="24">
         <v>384450</v>
       </c>
-      <c r="H34" s="27">
+      <c r="H35" s="24">
         <v>17716</v>
       </c>
-      <c r="I34" s="27">
+      <c r="I35" s="24">
         <v>742</v>
       </c>
-      <c r="J34" s="27">
+      <c r="J35" s="24">
         <v>0</v>
       </c>
-      <c r="K34" s="27">
+      <c r="K35" s="24">
         <v>2845</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A35" s="25" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A36" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B36" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="27">
+      <c r="C36" s="24">
         <v>2317135</v>
       </c>
-      <c r="D35" s="27">
+      <c r="D36" s="24">
         <v>2143352</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E36" s="24">
         <v>2011796</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F36" s="24">
         <v>120114</v>
       </c>
-      <c r="G35" s="27">
+      <c r="G36" s="24">
         <v>38860</v>
       </c>
-      <c r="H35" s="27">
+      <c r="H36" s="24">
         <v>8463</v>
       </c>
-      <c r="I35" s="27">
+      <c r="I36" s="24">
         <v>333</v>
       </c>
-      <c r="J35" s="27">
+      <c r="J36" s="24">
         <v>1</v>
       </c>
-      <c r="K35" s="27">
+      <c r="K36" s="24">
         <v>2645</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A36" s="28" t="s">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B37" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="30">
+      <c r="C37" s="27">
         <v>1617384</v>
       </c>
-      <c r="D36" s="30">
+      <c r="D37" s="27">
         <v>1464173</v>
       </c>
-      <c r="E36" s="30">
+      <c r="E37" s="27">
         <v>1418647</v>
       </c>
-      <c r="F36" s="30">
+      <c r="F37" s="27">
         <v>32832</v>
       </c>
-      <c r="G36" s="30">
+      <c r="G37" s="27">
         <v>50505</v>
       </c>
-      <c r="H36" s="30">
+      <c r="H37" s="27">
         <v>12298</v>
       </c>
-      <c r="I36" s="30">
+      <c r="I37" s="27">
         <v>41</v>
       </c>
-      <c r="J36" s="30">
+      <c r="J37" s="27">
         <v>0</v>
       </c>
-      <c r="K36" s="30">
+      <c r="K37" s="27">
         <v>355</v>
       </c>
     </row>

</xml_diff>